<commit_message>
lay 250 diem sang nhat
</commit_message>
<xml_diff>
--- a/Calibration_Value.xlsx
+++ b/Calibration_Value.xlsx
@@ -423,162 +423,162 @@
   <sheetData>
     <row r="2">
       <c r="B2" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F2" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="G2" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E3" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="G3" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C4" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="G4" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C5" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E5" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F5" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D6" t="n">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E6" t="n">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="F6" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C7" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E7" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F7" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G7" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C8" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F8" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="G8" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F9" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G9" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>